<commit_message>
Second Commit Logical Level Changes
</commit_message>
<xml_diff>
--- a/testTask/TestData/TestData.xlsx
+++ b/testTask/TestData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\API_Automation\testTask\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjain2\git\TestTask\testTask\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22918542-28ED-4B51-82C1-EB5F09DC670E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC3E49C-C152-457C-BF44-6AE23710A6E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{83908C0D-36BC-463F-B8B5-22638B583046}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>InlineParam</t>
   </si>
@@ -40,13 +40,48 @@
   <si>
     <t>false</t>
   </si>
+  <si>
+    <t>Carbon credits:true:2x larger image</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valuesToCompare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ExpectedFormat (NameValue:CanRelistValue:DescriptionValue)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,9 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,35 +430,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA1D91F-D052-4022-9AC7-D2A0EC5F0EDB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6327</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>